<commit_message>
mit kurven auf 1 und pbs 14 duokicated column fixed
</commit_message>
<xml_diff>
--- a/data/2024 BPS, Esf, food/14_days.xlsx
+++ b/data/2024 BPS, Esf, food/14_days.xlsx
@@ -58,7 +58,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -183,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -213,15 +213,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -541,10 +538,10 @@
     <col min="7" max="7" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -581,7 +578,7 @@
         <v>83.1111111111111</v>
       </c>
       <c r="D2" s="6">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="E2" s="6">
         <v>74.6666666666667</v>
@@ -596,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7">
         <v>0.01</v>
       </c>
@@ -607,7 +604,7 @@
         <v>93.3333333333334</v>
       </c>
       <c r="D3" s="6">
-        <v>93.3333333333334</v>
+        <v>98</v>
       </c>
       <c r="E3" s="6">
         <v>75.3333333333334</v>
@@ -618,7 +615,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7">
         <v>0.1</v>
       </c>
@@ -629,7 +626,7 @@
         <v>92.5</v>
       </c>
       <c r="D4" s="6">
-        <v>92.5</v>
+        <v>91</v>
       </c>
       <c r="E4" s="6">
         <v>55.3333333333334</v>
@@ -644,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -655,7 +652,7 @@
         <v>72.8888888888889</v>
       </c>
       <c r="D5" s="6">
-        <v>72.8888888888889</v>
+        <v>97.3333333333333</v>
       </c>
       <c r="E5" s="6">
         <v>78.2222222222222</v>
@@ -666,7 +663,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="8">
         <v>10</v>
       </c>
@@ -677,7 +674,7 @@
         <v>84</v>
       </c>
       <c r="D6" s="6">
-        <v>84</v>
+        <v>90.2222222222222</v>
       </c>
       <c r="E6" s="6">
         <v>66.2222222222222</v>
@@ -688,7 +685,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="8">
         <v>100</v>
       </c>
@@ -699,7 +696,7 @@
         <v>71.1111111111111</v>
       </c>
       <c r="D7" s="6">
-        <v>71.1111111111111</v>
+        <v>95.1111111111111</v>
       </c>
       <c r="E7" s="6">
         <v>63.5555555555556</v>
@@ -710,7 +707,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="8">
         <v>1000</v>
       </c>
@@ -721,7 +718,7 @@
         <v>40.4444444444444</v>
       </c>
       <c r="D8" s="6">
-        <v>40.4444444444444</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6">
         <v>40</v>
@@ -732,7 +729,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="8">
         <v>10000</v>
       </c>
@@ -754,7 +751,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="9"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>

</xml_diff>